<commit_message>
committing results parsed serially to avoid multithreading issues
</commit_message>
<xml_diff>
--- a/scalpel/typeinfer/evaluation/evaluation_outputs/drduh__macOS-Security-and-Privacy-Guide.xlsx
+++ b/scalpel/typeinfer/evaluation/evaluation_outputs/drduh__macOS-Security-and-Privacy-Guide.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -44,6 +44,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -70,7 +75,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -78,6 +83,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -443,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +512,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>{'any', 'plistlib.readPlistFromString'}</t>
+          <t>plistlib.readPlistFromString</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
@@ -528,7 +534,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>LoadPlist</t>
+          <t>GetPlistValue</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -538,12 +544,12 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>any</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>Win</t>
         </is>
       </c>
     </row>
@@ -560,22 +566,22 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>GetPlistValue</t>
+          <t>GetProgram</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Any</t>
+          <t>Tuple</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>{'bool', 'any'}</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>Win</t>
+          <t>any</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>Loss</t>
         </is>
       </c>
     </row>
@@ -592,22 +598,22 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>GetPlistValue</t>
+          <t>HashFile</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Any</t>
+          <t>str</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>bool</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>Win</t>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -624,20 +630,20 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>GetProgram</t>
+          <t>GetComment</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>Tuple</t>
+          <t>Any</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>{'Tuple[str]', 'any', 'Tuple[any]'}</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="inlineStr">
+          <t>any</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>Neutral</t>
         </is>
@@ -646,439 +652,57 @@
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
+          <t>Total comparisons:</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>GetProgram</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>Tuple</t>
-        </is>
+          <t>PyType Wins:</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>Tuple[str]</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
+          <t>Scalpel Wins:</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>HashFile</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
+      <c r="A8" s="2" t="inlineStr"/>
+      <c r="B8" s="2" t="inlineStr"/>
+      <c r="C8" s="2" t="inlineStr"/>
+      <c r="D8" s="2" t="inlineStr"/>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>{'str'}</t>
-        </is>
-      </c>
-      <c r="F8" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
+          <t>Scalpel Accuracy:</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>HashFile</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
+      <c r="A9" s="2" t="inlineStr"/>
+      <c r="B9" s="2" t="inlineStr"/>
+      <c r="C9" s="2" t="inlineStr"/>
+      <c r="D9" s="2" t="inlineStr"/>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="F9" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>GetComment</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>Any</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>{'any'}</t>
-        </is>
-      </c>
-      <c r="F10" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>GetComment</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>Any</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="inlineStr">
-        <is>
-          <t>any</t>
-        </is>
-      </c>
-      <c r="F11" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>LoadPlist</t>
-        </is>
-      </c>
-      <c r="D12" s="2" t="inlineStr">
-        <is>
-          <t>Any</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="inlineStr">
-        <is>
-          <t>list</t>
-        </is>
-      </c>
-      <c r="F12" s="3" t="inlineStr">
-        <is>
-          <t>Win</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>GetPlistValue</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>Any</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="inlineStr">
-        <is>
-          <t>any</t>
-        </is>
-      </c>
-      <c r="F13" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>GetPlistValue</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="inlineStr">
-        <is>
-          <t>Any</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="inlineStr">
-        <is>
-          <t>any</t>
-        </is>
-      </c>
-      <c r="F14" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>GetProgram</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>Any</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="inlineStr">
-        <is>
-          <t>any</t>
-        </is>
-      </c>
-      <c r="F15" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>HashFile</t>
-        </is>
-      </c>
-      <c r="D16" s="2" t="inlineStr">
-        <is>
-          <t>Any</t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="inlineStr">
-        <is>
-          <t>list</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>Win</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>GetComment</t>
-        </is>
-      </c>
-      <c r="D17" s="2" t="inlineStr">
-        <is>
-          <t>Any</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="inlineStr">
-        <is>
-          <t>any</t>
-        </is>
-      </c>
-      <c r="F17" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>drduh__macOS-Security-and-Privacy-Guide</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>read_launch_plists.py</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>GetComment</t>
-        </is>
-      </c>
-      <c r="D18" s="2" t="inlineStr">
-        <is>
-          <t>Any</t>
-        </is>
-      </c>
-      <c r="E18" s="2" t="inlineStr">
-        <is>
-          <t>any</t>
-        </is>
-      </c>
-      <c r="F18" s="4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>Total comparisons:</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t>PyType Wins:</t>
-        </is>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="inlineStr">
-        <is>
-          <t>Scalpel Wins:</t>
-        </is>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr"/>
-      <c r="B20" s="2" t="inlineStr"/>
-      <c r="C20" s="2" t="inlineStr"/>
-      <c r="D20" s="2" t="inlineStr"/>
-      <c r="E20" s="2" t="inlineStr">
-        <is>
-          <t>Scalpel Accuracy:</t>
-        </is>
-      </c>
-      <c r="F20" s="2" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr"/>
-      <c r="B21" s="2" t="inlineStr"/>
-      <c r="C21" s="2" t="inlineStr"/>
-      <c r="D21" s="2" t="inlineStr"/>
-      <c r="E21" s="2" t="inlineStr">
-        <is>
           <t>Accuracy vs PyType</t>
         </is>
       </c>
-      <c r="F21" s="2" t="n">
-        <v>100</v>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>133.32999999999998%</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>